<commit_message>
Document for presentation and update excel
</commit_message>
<xml_diff>
--- a/time spent.xlsx
+++ b/time spent.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmlozanoo\Documents\GitHub\PR-25-SDG-Interview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chema\Documents\GitHub\PR-25-SDG-Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58951C6B-D1EA-4CC8-AAEF-655E48E1455D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD8D602-AAF6-4AEA-B2AF-4CDB2A2A1D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{51FA7B74-6C82-4C33-A93D-C38C06450FA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{51FA7B74-6C82-4C33-A93D-C38C06450FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>description</t>
   </si>
@@ -71,7 +71,10 @@
     <t>time spend(min)</t>
   </si>
   <si>
-    <t>total (10 hours and 55 minutes)</t>
+    <t>total (11 hours and 25 minutes)</t>
+  </si>
+  <si>
+    <t>review before presentation</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -467,13 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AC3684-6DC0-41A1-A552-DA8F20BAB909}">
-  <dimension ref="B5:F17"/>
+  <dimension ref="B5:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
@@ -530,7 +533,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="9">
-        <f t="shared" ref="F7:F16" si="0">(D7-C7)*60*24</f>
+        <f t="shared" ref="F7:F17" si="0">(D7-C7)*60*24</f>
         <v>30.000000000000053</v>
       </c>
     </row>
@@ -697,15 +700,33 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11" t="s">
+      <c r="B17" s="2">
+        <v>45165</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>29.999999999999893</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="12">
-        <f>SUM(F6:F16)</f>
-        <v>655.00000000000023</v>
+      <c r="F18" s="12">
+        <f>SUM(F6:F17)</f>
+        <v>685.00000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>